<commit_message>
start of nsga2 for 100 generation with constraints
</commit_message>
<xml_diff>
--- a/examples/magnetics/reluctance_machine/supplementary/parameters.xlsx
+++ b/examples/magnetics/reluctance_machine/supplementary/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Respositories\py2femm\examples\magnetics\reluctance_machine\supplementary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089BD109-D678-4FFD-B6FE-403C720E4719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E428FEBD-DD23-4793-9E05-0CCAD8BDD3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25365" yWindow="465" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Parameter</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Level5</t>
+  </si>
+  <si>
+    <t>NSGA2</t>
   </si>
 </sst>
 </file>
@@ -471,10 +474,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB46AD7-974B-48E2-B8C2-C8A7465E005C}">
-  <dimension ref="A1:AA9"/>
+  <dimension ref="A1:AA18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,6 +703,95 @@
         <v>2.5</v>
       </c>
     </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>90</v>
+      </c>
+      <c r="D14">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>1.5</v>
+      </c>
+      <c r="D18">
+        <v>2.5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:AA1"/>

</xml_diff>